<commit_message>
added some nonmilitary industries. finished working draft of r script for plots and tables.
</commit_message>
<xml_diff>
--- a/data/source/industries/aircraft_and_parts.xlsx
+++ b/data/source/industries/aircraft_and_parts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex\coding_projects\bls_data\data\source\industries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA9AC10-E8F1-4C19-8B22-F67F06083027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22FD12C3-2800-4894-9D0C-B3E9E299EAD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31950" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve"> Year</t>
   </si>
@@ -78,9 +78,6 @@
   </si>
   <si>
     <t>n/a</t>
-  </si>
-  <si>
-    <t>72.7  *</t>
   </si>
 </sst>
 </file>
@@ -398,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,7 +455,7 @@
         <v>13</v>
       </c>
       <c r="D2">
-        <v>93</v>
+        <v>515.29999999999995</v>
       </c>
       <c r="E2">
         <v>101.25</v>
@@ -498,12 +495,21 @@
       <c r="C3">
         <v>107.1</v>
       </c>
+      <c r="D3">
+        <v>476.2</v>
+      </c>
+      <c r="E3">
+        <v>106.63</v>
+      </c>
       <c r="F3">
         <v>2.62</v>
       </c>
       <c r="G3">
         <v>40.700000000000003</v>
       </c>
+      <c r="H3">
+        <v>2.1</v>
+      </c>
       <c r="I3">
         <v>2.2999999999999998</v>
       </c>
@@ -512,6 +518,9 @@
       </c>
       <c r="K3">
         <v>3.2</v>
+      </c>
+      <c r="L3">
+        <v>1.2</v>
       </c>
       <c r="M3">
         <v>1.5</v>
@@ -527,8 +536,11 @@
       <c r="C4">
         <v>93</v>
       </c>
+      <c r="D4">
+        <v>407.4</v>
+      </c>
       <c r="E4">
-        <v>106.63</v>
+        <v>110.43</v>
       </c>
       <c r="F4">
         <v>2.7</v>
@@ -537,7 +549,7 @@
         <v>40.9</v>
       </c>
       <c r="H4">
-        <v>2.1</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I4">
         <v>2.4</v>
@@ -549,7 +561,7 @@
         <v>3.3</v>
       </c>
       <c r="L4">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="M4">
         <v>1.7</v>
@@ -566,7 +578,31 @@
         <v>88.8</v>
       </c>
       <c r="D5">
-        <v>88.8</v>
+        <v>351.7</v>
+      </c>
+      <c r="E5">
+        <v>114.68</v>
+      </c>
+      <c r="F5">
+        <v>2.77</v>
+      </c>
+      <c r="G5">
+        <v>41.4</v>
+      </c>
+      <c r="H5">
+        <v>2.5</v>
+      </c>
+      <c r="I5">
+        <v>2.8</v>
+      </c>
+      <c r="J5">
+        <v>1.7</v>
+      </c>
+      <c r="K5">
+        <v>2.6</v>
+      </c>
+      <c r="L5">
+        <v>0.9</v>
       </c>
       <c r="M5">
         <v>1.3</v>
@@ -582,28 +618,34 @@
       <c r="C6">
         <v>92.1</v>
       </c>
+      <c r="D6">
+        <v>356.4</v>
+      </c>
       <c r="E6">
-        <v>110.43</v>
+        <v>119.97</v>
       </c>
       <c r="F6">
-        <v>2.77</v>
+        <v>2.87</v>
       </c>
       <c r="G6">
-        <v>41.4</v>
+        <v>41.8</v>
       </c>
       <c r="H6">
-        <v>2.2000000000000002</v>
+        <v>2.9</v>
       </c>
       <c r="I6">
-        <v>2.8</v>
+        <v>2.9</v>
       </c>
       <c r="J6">
-        <v>1.7</v>
+        <v>2.1</v>
       </c>
       <c r="K6">
-        <v>2.6</v>
+        <v>2.5</v>
       </c>
       <c r="L6">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="M6">
         <v>1</v>
       </c>
     </row>
@@ -615,22 +657,37 @@
         <v>639.20000000000005</v>
       </c>
       <c r="C7">
-        <v>883</v>
+        <v>88.3</v>
       </c>
       <c r="D7">
-        <v>92.1</v>
+        <v>358.2</v>
+      </c>
+      <c r="E7">
+        <v>122.43</v>
       </c>
       <c r="F7">
-        <v>2.87</v>
+        <v>2.95</v>
       </c>
       <c r="G7">
-        <v>41.8</v>
+        <v>41.5</v>
+      </c>
+      <c r="H7">
+        <v>2.6</v>
       </c>
       <c r="I7">
-        <v>2.9</v>
+        <v>2.4</v>
       </c>
       <c r="J7">
-        <v>2.1</v>
+        <v>1.7</v>
+      </c>
+      <c r="K7">
+        <v>2.5</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -643,26 +700,35 @@
       <c r="C8">
         <v>80.3</v>
       </c>
+      <c r="D8">
+        <v>352.7</v>
+      </c>
+      <c r="E8">
+        <v>125.03</v>
+      </c>
       <c r="F8">
-        <v>2.95</v>
+        <v>3.02</v>
       </c>
       <c r="G8">
-        <v>41.5</v>
+        <v>41.4</v>
+      </c>
+      <c r="H8">
+        <v>2.5</v>
       </c>
       <c r="I8">
-        <v>2.4</v>
+        <v>2.1</v>
       </c>
       <c r="J8">
-        <v>1.7</v>
+        <v>1.4</v>
       </c>
       <c r="K8">
-        <v>2.5</v>
+        <v>2.6</v>
       </c>
       <c r="L8">
         <v>0.9</v>
       </c>
       <c r="M8">
-        <v>1</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -676,28 +742,34 @@
         <v>82.7</v>
       </c>
       <c r="D9">
-        <v>883</v>
+        <v>339.2</v>
       </c>
       <c r="E9">
-        <v>114.68</v>
+        <v>131.88</v>
       </c>
       <c r="F9">
-        <v>3.02</v>
+        <v>3.14</v>
       </c>
       <c r="G9">
-        <v>41.4</v>
+        <v>42</v>
       </c>
       <c r="H9">
+        <v>3.3</v>
+      </c>
+      <c r="I9">
+        <v>3.2</v>
+      </c>
+      <c r="J9">
         <v>2.5</v>
       </c>
-      <c r="I9">
-        <v>2.1</v>
-      </c>
-      <c r="J9">
-        <v>1.4</v>
+      <c r="K9">
+        <v>2.2999999999999998</v>
       </c>
       <c r="L9">
         <v>1.1000000000000001</v>
+      </c>
+      <c r="M9">
+        <v>0.7</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -710,26 +782,35 @@
       <c r="C10">
         <v>107.3</v>
       </c>
+      <c r="D10">
+        <v>402.5</v>
+      </c>
+      <c r="E10">
+        <v>143.32</v>
+      </c>
       <c r="F10">
-        <v>3.14</v>
+        <v>3.31</v>
       </c>
       <c r="G10">
-        <v>42</v>
+        <v>43.3</v>
+      </c>
+      <c r="H10">
+        <v>5</v>
       </c>
       <c r="I10">
-        <v>3.2</v>
+        <v>4.2</v>
       </c>
       <c r="J10">
-        <v>2.5</v>
+        <v>3.6</v>
       </c>
       <c r="K10">
-        <v>2.5</v>
+        <v>2.6</v>
       </c>
       <c r="L10">
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="M10">
-        <v>1.1000000000000001</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -743,28 +824,34 @@
         <v>127</v>
       </c>
       <c r="D11">
-        <v>80.3</v>
+        <v>489.5</v>
       </c>
       <c r="E11">
-        <v>119.97</v>
+        <v>146.97</v>
       </c>
       <c r="F11">
-        <v>3.31</v>
+        <v>3.45</v>
       </c>
       <c r="G11">
-        <v>43.3</v>
+        <v>42.6</v>
       </c>
       <c r="H11">
-        <v>2.9</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="I11">
-        <v>4.2</v>
+        <v>3.1</v>
       </c>
       <c r="J11">
-        <v>3.6</v>
+        <v>2.6</v>
+      </c>
+      <c r="K11">
+        <v>2.7</v>
       </c>
       <c r="L11">
-        <v>0.9</v>
+        <v>1.6</v>
+      </c>
+      <c r="M11">
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -777,26 +864,35 @@
       <c r="C12">
         <v>128.4</v>
       </c>
+      <c r="D12">
+        <v>519.79999999999995</v>
+      </c>
+      <c r="E12">
+        <v>152.04</v>
+      </c>
       <c r="F12">
-        <v>3.45</v>
+        <v>3.62</v>
       </c>
       <c r="G12">
-        <v>42.6</v>
+        <v>42</v>
+      </c>
+      <c r="H12">
+        <v>3.8</v>
       </c>
       <c r="I12">
-        <v>3.1</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="J12">
-        <v>2.6</v>
+        <v>1.8</v>
       </c>
       <c r="K12">
-        <v>2.6</v>
+        <v>2.7</v>
       </c>
       <c r="L12">
-        <v>1.1000000000000001</v>
+        <v>1.5</v>
       </c>
       <c r="M12">
-        <v>1.2</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -810,31 +906,34 @@
         <v>119.1</v>
       </c>
       <c r="D13">
-        <v>82.7</v>
+        <v>485.6</v>
       </c>
       <c r="E13">
-        <v>122.43</v>
+        <v>161.35</v>
       </c>
       <c r="F13">
-        <v>3.62</v>
+        <v>3.86</v>
       </c>
       <c r="G13">
-        <v>42</v>
+        <v>41.8</v>
       </c>
       <c r="H13">
-        <v>2.6</v>
+        <v>3.4</v>
       </c>
       <c r="I13">
-        <v>2.2999999999999998</v>
+        <v>2</v>
       </c>
       <c r="J13">
-        <v>1.8</v>
+        <v>1.4</v>
       </c>
       <c r="K13">
-        <v>2.2999999999999998</v>
+        <v>2.8</v>
       </c>
       <c r="L13">
-        <v>1.6</v>
+        <v>1.3</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -848,22 +947,34 @@
         <v>94.6</v>
       </c>
       <c r="D14">
-        <v>107.3</v>
+        <v>421.9</v>
+      </c>
+      <c r="E14">
+        <v>168.51</v>
       </c>
       <c r="F14">
-        <v>3.86</v>
+        <v>4.1100000000000003</v>
       </c>
       <c r="G14">
-        <v>41.8</v>
+        <v>41</v>
+      </c>
+      <c r="H14">
+        <v>2.7</v>
+      </c>
+      <c r="I14">
+        <v>1.4</v>
       </c>
       <c r="J14">
-        <v>1.4</v>
+        <v>0.7</v>
+      </c>
+      <c r="K14">
+        <v>3.5</v>
       </c>
       <c r="L14">
-        <v>1.6</v>
+        <v>0.8</v>
       </c>
       <c r="M14">
-        <v>0.7</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -876,29 +987,35 @@
       <c r="C15">
         <v>72.7</v>
       </c>
+      <c r="D15">
+        <v>321.7</v>
+      </c>
       <c r="E15">
-        <v>125.03</v>
+        <v>175.82</v>
       </c>
       <c r="F15">
-        <v>4.1100000000000003</v>
+        <v>4.32</v>
       </c>
       <c r="G15">
-        <v>41</v>
+        <v>40.700000000000003</v>
       </c>
       <c r="H15">
-        <v>2.5</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="I15">
-        <v>2</v>
+        <v>1.7</v>
       </c>
       <c r="J15">
         <v>0.7</v>
       </c>
       <c r="K15">
-        <v>2.6</v>
+        <v>3</v>
       </c>
       <c r="L15">
-        <v>1.5</v>
+        <v>0.6</v>
+      </c>
+      <c r="M15">
+        <v>1.9</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -912,13 +1029,34 @@
         <v>70.7</v>
       </c>
       <c r="D16">
-        <v>127</v>
+        <v>270</v>
+      </c>
+      <c r="E16">
+        <v>193.44</v>
+      </c>
+      <c r="F16">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="G16">
+        <v>41.6</v>
+      </c>
+      <c r="H16">
+        <v>3</v>
+      </c>
+      <c r="I16">
+        <v>2</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>2</v>
       </c>
       <c r="L16">
-        <v>1.3</v>
+        <v>0.7</v>
       </c>
       <c r="M16">
-        <v>0.3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -931,26 +1069,35 @@
       <c r="C17">
         <v>77.900000000000006</v>
       </c>
+      <c r="D17">
+        <v>287.3</v>
+      </c>
       <c r="E17">
-        <v>131.88</v>
+        <v>207.92</v>
       </c>
       <c r="F17">
-        <v>4.32</v>
+        <v>5.01</v>
+      </c>
+      <c r="G17">
+        <v>41.5</v>
       </c>
       <c r="H17">
-        <v>3.3</v>
+        <v>3.4</v>
       </c>
       <c r="I17">
-        <v>1.4</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="J17">
+        <v>1.5</v>
+      </c>
+      <c r="K17">
+        <v>2.1</v>
+      </c>
+      <c r="L17">
+        <v>0.9</v>
+      </c>
+      <c r="M17">
         <v>0.7</v>
-      </c>
-      <c r="K17">
-        <v>2.7</v>
-      </c>
-      <c r="L17">
-        <v>0.8</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -964,208 +1111,34 @@
         <v>83.6</v>
       </c>
       <c r="D18">
-        <v>128.4</v>
+        <v>295.10000000000002</v>
       </c>
       <c r="E18">
-        <v>143.32</v>
+        <v>218.7</v>
       </c>
       <c r="F18">
-        <v>4.6500000000000004</v>
+        <v>5.4</v>
       </c>
       <c r="G18">
-        <v>40.700000000000003</v>
+        <v>40.5</v>
+      </c>
+      <c r="H18">
+        <v>3.2</v>
+      </c>
+      <c r="I18">
+        <v>2.1</v>
       </c>
       <c r="J18">
-        <v>1</v>
+        <v>1.5</v>
+      </c>
+      <c r="K18">
+        <v>1.9</v>
+      </c>
+      <c r="L18">
+        <v>0.8</v>
       </c>
       <c r="M18">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F19">
-        <v>5.01</v>
-      </c>
-      <c r="G19">
-        <v>41.6</v>
-      </c>
-      <c r="H19">
-        <v>5</v>
-      </c>
-      <c r="I19">
-        <v>1.7</v>
-      </c>
-      <c r="J19">
-        <v>1.5</v>
-      </c>
-      <c r="K19">
-        <v>2.7</v>
-      </c>
-      <c r="L19">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D20">
-        <v>119.1</v>
-      </c>
-      <c r="E20">
-        <v>146.97</v>
-      </c>
-      <c r="F20">
-        <v>5.4</v>
-      </c>
-      <c r="H20">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="J20">
-        <v>1.5</v>
-      </c>
-      <c r="L20">
-        <v>0.7</v>
-      </c>
-      <c r="M20">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="G21">
-        <v>41.5</v>
-      </c>
-      <c r="I21">
-        <v>2</v>
-      </c>
-      <c r="K21">
-        <v>2.8</v>
-      </c>
-      <c r="L21">
-        <v>0.9</v>
-      </c>
-      <c r="M21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D22">
-        <v>94.6</v>
-      </c>
-      <c r="E22">
-        <v>152.04</v>
-      </c>
-      <c r="G22">
-        <v>40.5</v>
-      </c>
-      <c r="H22">
-        <v>3.8</v>
-      </c>
-      <c r="I22">
-        <v>2.2999999999999998</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I23">
-        <v>2.1</v>
-      </c>
-      <c r="K23">
-        <v>3.5</v>
-      </c>
-      <c r="L23">
-        <v>0.8</v>
-      </c>
-      <c r="M23">
-        <v>2.2000000000000002</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E24">
-        <v>161.35</v>
-      </c>
-      <c r="H24">
-        <v>3.4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D25" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E26">
-        <v>168.51</v>
-      </c>
-      <c r="H26">
-        <v>2.7</v>
-      </c>
-      <c r="K26">
-        <v>3</v>
-      </c>
-      <c r="M26">
-        <v>1.9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D27">
-        <v>70.7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E28">
-        <v>175.82</v>
-      </c>
-      <c r="K28">
-        <v>2</v>
-      </c>
-      <c r="M28">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D29">
-        <v>77.900000000000006</v>
-      </c>
-      <c r="E29">
-        <v>193.44</v>
-      </c>
-      <c r="H29">
-        <v>2.2999999999999998</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H30">
-        <v>3</v>
-      </c>
-      <c r="K30">
-        <v>2.1</v>
-      </c>
-      <c r="M30">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D31">
-        <v>83.6</v>
-      </c>
-      <c r="E31">
-        <v>207.92</v>
-      </c>
-      <c r="H31">
-        <v>3.4</v>
-      </c>
-      <c r="K31">
-        <v>1.9</v>
-      </c>
-      <c r="M31">
         <v>0.5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E32">
-        <v>218.7</v>
-      </c>
-    </row>
-    <row r="33" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H33">
-        <v>3.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>